<commit_message>
Added function to write headings before writing anything else to the Excel file
</commit_message>
<xml_diff>
--- a/Expenses01.xlsx
+++ b/Expenses01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="46">
   <si>
     <t xml:space="preserve">01 Oct, 2017  </t>
   </si>
@@ -22,25 +22,136 @@
     <t>Electronics &amp; Electrical</t>
   </si>
   <si>
-    <t>Packaging Tapes</t>
-  </si>
-  <si>
-    <t>Pune, India</t>
+    <t>Teflon sealing Tapes</t>
+  </si>
+  <si>
+    <t>Bhubaneswar, India</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>40-50</t>
-  </si>
-  <si>
-    <t>Industrial Plant &amp; Machinery</t>
-  </si>
-  <si>
-    <t>Manual Fusing Machines</t>
-  </si>
-  <si>
-    <t>Nashik, India</t>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Yufeng E Rickshaw Motor</t>
+  </si>
+  <si>
+    <t>Delhi, India</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>For E Rickshaw</t>
+  </si>
+  <si>
+    <t>Power Touch Inverter Tubular Battery</t>
+  </si>
+  <si>
+    <t>Betul, India</t>
+  </si>
+  <si>
+    <t>Pieces</t>
+  </si>
+  <si>
+    <t>Aadhar Kit</t>
+  </si>
+  <si>
+    <t>Gurgaon, India</t>
+  </si>
+  <si>
+    <t>CCTV Camera</t>
+  </si>
+  <si>
+    <t>Dhaka, Bangladesh</t>
+  </si>
+  <si>
+    <t>Canon EOS DSLR Body</t>
+  </si>
+  <si>
+    <t>Nagapattinam, India</t>
+  </si>
+  <si>
+    <t>Latest Jhoomer Light</t>
+  </si>
+  <si>
+    <t>Kota, India</t>
+  </si>
+  <si>
+    <t>LED Raw Material</t>
+  </si>
+  <si>
+    <t>Anakapalli, India</t>
+  </si>
+  <si>
+    <t>Nos</t>
+  </si>
+  <si>
+    <t>Gorilla Ceiling Fan and Blade less Fan</t>
+  </si>
+  <si>
+    <t>Vijayawada, India</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Crystal Oscillator</t>
+  </si>
+  <si>
+    <t>Agra, India</t>
+  </si>
+  <si>
+    <t>Electric Fan Box</t>
+  </si>
+  <si>
+    <t>Amritsar, India</t>
+  </si>
+  <si>
+    <t>Bonfiglioli Geared Motor</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Spike Guard</t>
+  </si>
+  <si>
+    <t>Navi Mumbai, India</t>
+  </si>
+  <si>
+    <t>Laptop Rentals Service</t>
+  </si>
+  <si>
+    <t>New Delhi, India</t>
+  </si>
+  <si>
+    <t>4 GB</t>
+  </si>
+  <si>
+    <t>Water Purifier Service</t>
+  </si>
+  <si>
+    <t>Bhopal, India</t>
+  </si>
+  <si>
+    <t>Cable Route Locator</t>
+  </si>
+  <si>
+    <t>Commercial Electrical Contractor</t>
+  </si>
+  <si>
+    <t>Mumbai, India</t>
+  </si>
+  <si>
+    <t>Havells Solar DC Wire</t>
+  </si>
+  <si>
+    <t>Steel Double Interlock Flexible Conduit Pipe</t>
+  </si>
+  <si>
+    <t>Bengaluru, India</t>
   </si>
 </sst>
 </file>
@@ -372,41 +483,584 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:K3"/>
+  <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="2" spans="2:11">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="3" spans="2:11">
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
       <c r="J3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>